<commit_message>
new changes are added
</commit_message>
<xml_diff>
--- a/Books.xlsx
+++ b/Books.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="testcases for MyAccount section" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="143">
   <si>
     <t>Steps</t>
   </si>
@@ -1059,8 +1059,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A2:L12"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12:XFD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1679,7 +1679,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A4:L18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="107" zoomScaleNormal="107" workbookViewId="0">
+    <sheetView topLeftCell="A2" zoomScale="107" zoomScaleNormal="107" workbookViewId="0">
       <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>

</xml_diff>